<commit_message>
Implement category-based extraction, source evidence with PDF page tracking, and preserve field order
</commit_message>
<xml_diff>
--- a/항목파일_0129.xlsx
+++ b/항목파일_0129.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\reportanalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECA8E92-63FF-422A-BE4E-B14E47358C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCA798F-3375-4650-8F3C-3BF4C6032B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{97C7DBA4-68FA-46C9-A20C-1CFFF3F16A6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="99">
   <si>
     <t>필드명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -398,6 +398,26 @@
   </si>
   <si>
     <t>찾아가는 컨설팅 참여할 경우 참여하는 인원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충분한 운영시간 및 일수 보장 및 추가 인력 배치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요 맞춤 교육·돌봄의 질 제고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교사 대 영유아수 비율 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교사 전문성 및 역량 강화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분야</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -436,12 +456,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -450,11 +485,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -791,739 +829,890 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD1129C-7BFD-41EE-B55B-05ACA5588995}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.75" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.375" customWidth="1"/>
+    <col min="1" max="1" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.75" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
       <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
       <c r="D17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>31</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>26</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>31</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>41</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>42</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>41</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>42</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>41</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>42</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>41</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>42</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>42</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>41</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>42</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>41</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>42</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>63</v>
       </c>
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
       <c r="D36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>65</v>
       </c>
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
       <c r="D37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>67</v>
       </c>
-      <c r="C38" t="s">
-        <v>16</v>
-      </c>
       <c r="D38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>69</v>
       </c>
-      <c r="C39" t="s">
-        <v>16</v>
-      </c>
       <c r="D39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>26</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>73</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>26</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>74</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>42</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>76</v>
       </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
       <c r="D43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>77</v>
       </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
       <c r="D44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>78</v>
       </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
       <c r="D45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>80</v>
       </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
       <c r="D46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>82</v>
       </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
       <c r="D47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>84</v>
       </c>
-      <c r="C48" t="s">
-        <v>16</v>
-      </c>
       <c r="D48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>90</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>26</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>91</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>26</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>92</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>26</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>93</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>26</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>